<commit_message>
fix: :bug: Se corrige error en el nombre de la persona quien realizo la orden de compra
Se corrigio error que las requisiciones salian con el nombre de maquinaria para las ordenes de compra de planeación
</commit_message>
<xml_diff>
--- a/src/ExcelsStorageRequis/plantillas/planeacion/Factura.xlsx
+++ b/src/ExcelsStorageRequis/plantillas/planeacion/Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBT\Documents\TBTapp\tbt-app\src\ExcelsStorageRequis\plantillas\planeacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725A13E5-8F17-4E81-8C24-BF35784F6913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EACA1F-01F6-417C-98F3-3FABF7F0816B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{23728274-58D1-446B-AD76-22B014C06C12}"/>
   </bookViews>
   <sheets>
     <sheet name="requi" sheetId="1" r:id="rId1"/>
@@ -292,12 +292,6 @@
     <t xml:space="preserve">N° PARTE </t>
   </si>
   <si>
-    <t>Superintendente de Maquinaria</t>
-  </si>
-  <si>
-    <t>Ing. Othoniel Gonzalez Ruiz</t>
-  </si>
-  <si>
     <t>CONTRAPAGO</t>
   </si>
   <si>
@@ -305,6 +299,12 @@
   </si>
   <si>
     <t xml:space="preserve">L.C. MARY CARMEN BAUTISTA </t>
+  </si>
+  <si>
+    <t>L.C. Mary Carmen Bautista</t>
+  </si>
+  <si>
+    <t>Auxiliar Administrativo</t>
   </si>
 </sst>
 </file>
@@ -1808,6 +1808,114 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1817,121 +1925,181 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="82" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1987,174 +2155,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="67" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="73" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="74" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="76" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="75" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="77" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="78" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="71" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="62" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="63" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="64" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="82" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="43" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="44" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="51" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="47" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="52" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2228,22 +2228,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>273843</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>916980</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>12107</xdr:rowOff>
+      <xdr:colOff>897454</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>152599</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53AF49CC-C10B-8AEE-7FE5-F28BCC31FC95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4ADCFD1F-CB59-4A4A-A5F5-9BE5BB1C73B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2265,8 +2265,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="440531" y="6393658"/>
-          <a:ext cx="1428949" cy="1428949"/>
+          <a:off x="409575" y="8086725"/>
+          <a:ext cx="1478479" cy="1467049"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2780,98 +2780,98 @@
   </sheetPr>
   <dimension ref="B2:U45"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="U63" sqref="U63:U64"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5703125" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" customWidth="1"/>
-    <col min="19" max="20" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5546875" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" customWidth="1"/>
+    <col min="18" max="18" width="9.88671875" customWidth="1"/>
+    <col min="19" max="20" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="20.25" customHeight="1">
-      <c r="F2" s="159" t="s">
+      <c r="F2" s="134" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159"/>
-      <c r="I2" s="159"/>
-      <c r="J2" s="159"/>
-      <c r="K2" s="159"/>
-      <c r="L2" s="159"/>
-      <c r="M2" s="159"/>
-      <c r="N2" s="159"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
       <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:15" ht="35.25" customHeight="1">
-      <c r="F3" s="160" t="s">
+      <c r="F3" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
-      <c r="L3" s="160"/>
-      <c r="M3" s="160"/>
-      <c r="N3" s="160"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="135"/>
       <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:15" ht="7.5" customHeight="1"/>
-    <row r="5" spans="2:15" ht="15.75">
+    <row r="5" spans="2:15" ht="15.6">
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="161"/>
-      <c r="I5" s="161"/>
-      <c r="J5" s="161"/>
-      <c r="K5" s="162" t="s">
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="162"/>
-      <c r="M5" s="162"/>
-      <c r="N5" s="163"/>
+      <c r="L5" s="137"/>
+      <c r="M5" s="137"/>
+      <c r="N5" s="138"/>
       <c r="O5" s="29"/>
     </row>
-    <row r="6" spans="2:15" ht="15.75">
-      <c r="D6" s="161"/>
-      <c r="E6" s="161"/>
-      <c r="F6" s="161"/>
-      <c r="G6" s="161"/>
-      <c r="H6" s="161"/>
-      <c r="I6" s="161"/>
-      <c r="J6" s="161"/>
+    <row r="6" spans="2:15" ht="15.6">
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
       <c r="K6" s="28"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="164"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="165"/>
-      <c r="F7" s="165"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
       <c r="H7" s="27" t="s">
         <v>38</v>
       </c>
@@ -2879,17 +2879,17 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="166" t="s">
+      <c r="M7" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="166"/>
-      <c r="O7" s="166"/>
+      <c r="N7" s="141"/>
+      <c r="O7" s="141"/>
     </row>
     <row r="8" spans="2:15" ht="12.75" customHeight="1">
       <c r="B8" s="25"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
       <c r="H8" s="22"/>
       <c r="I8" s="21" t="s">
         <v>36</v>
@@ -2899,10 +2899,10 @@
       <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
+      <c r="C9" s="139"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="139"/>
+      <c r="F9" s="139"/>
       <c r="H9" s="22"/>
       <c r="I9" s="21" t="s">
         <v>34</v>
@@ -2927,10 +2927,10 @@
       <c r="B11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="167"/>
-      <c r="D11" s="167"/>
-      <c r="E11" s="167"/>
-      <c r="F11" s="167"/>
+      <c r="C11" s="143"/>
+      <c r="D11" s="143"/>
+      <c r="E11" s="143"/>
+      <c r="F11" s="143"/>
       <c r="G11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2962,52 +2962,52 @@
       </c>
     </row>
     <row r="17" spans="2:21">
-      <c r="B17" s="150" t="s">
+      <c r="B17" s="154" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="152" t="s">
+      <c r="D17" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="153"/>
-      <c r="F17" s="153"/>
-      <c r="G17" s="153"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="152" t="s">
+      <c r="E17" s="145"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="146"/>
+      <c r="I17" s="144" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="150" t="s">
+      <c r="J17" s="154" t="s">
         <v>19</v>
       </c>
-      <c r="K17" s="150" t="s">
+      <c r="K17" s="154" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="152" t="s">
+      <c r="L17" s="144" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="153"/>
-      <c r="N17" s="153"/>
-      <c r="O17" s="154"/>
+      <c r="M17" s="145"/>
+      <c r="N17" s="145"/>
+      <c r="O17" s="146"/>
     </row>
     <row r="18" spans="2:21">
-      <c r="B18" s="151"/>
+      <c r="B18" s="155"/>
       <c r="C18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="155"/>
-      <c r="E18" s="156"/>
-      <c r="F18" s="156"/>
-      <c r="G18" s="156"/>
-      <c r="H18" s="157"/>
-      <c r="I18" s="155"/>
-      <c r="J18" s="151"/>
-      <c r="K18" s="151"/>
-      <c r="L18" s="155"/>
-      <c r="M18" s="156"/>
-      <c r="N18" s="156"/>
-      <c r="O18" s="157"/>
+      <c r="D18" s="147"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="149"/>
+      <c r="I18" s="147"/>
+      <c r="J18" s="155"/>
+      <c r="K18" s="155"/>
+      <c r="L18" s="147"/>
+      <c r="M18" s="148"/>
+      <c r="N18" s="148"/>
+      <c r="O18" s="149"/>
     </row>
     <row r="19" spans="2:21">
       <c r="B19" s="18"/>
@@ -3030,23 +3030,23 @@
         <v>1</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="168"/>
-      <c r="E20" s="169"/>
-      <c r="F20" s="169"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="170"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="151"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="152"/>
       <c r="I20" s="17"/>
       <c r="J20" s="34"/>
       <c r="K20" s="16"/>
       <c r="L20" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="M20" s="144"/>
-      <c r="N20" s="144"/>
-      <c r="O20" s="145"/>
+      <c r="M20" s="160"/>
+      <c r="N20" s="160"/>
+      <c r="O20" s="161"/>
       <c r="R20" s="1"/>
-      <c r="T20" s="143"/>
-      <c r="U20" s="143"/>
+      <c r="T20" s="156"/>
+      <c r="U20" s="156"/>
     </row>
     <row r="21" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="12">
@@ -3054,24 +3054,24 @@
         <v>2</v>
       </c>
       <c r="C21" s="12"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="138"/>
-      <c r="H21" s="139"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="158"/>
+      <c r="F21" s="158"/>
+      <c r="G21" s="158"/>
+      <c r="H21" s="159"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="146"/>
-      <c r="N21" s="146"/>
-      <c r="O21" s="147"/>
+      <c r="M21" s="162"/>
+      <c r="N21" s="162"/>
+      <c r="O21" s="163"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="1"/>
-      <c r="T21" s="143"/>
-      <c r="U21" s="143"/>
+      <c r="T21" s="156"/>
+      <c r="U21" s="156"/>
     </row>
     <row r="22" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="12">
@@ -3079,25 +3079,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="12"/>
-      <c r="D22" s="137"/>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="139"/>
+      <c r="D22" s="157"/>
+      <c r="E22" s="158"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
+      <c r="H22" s="159"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="146"/>
-      <c r="N22" s="146"/>
-      <c r="O22" s="146"/>
+      <c r="M22" s="162"/>
+      <c r="N22" s="162"/>
+      <c r="O22" s="162"/>
       <c r="P22" s="33"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="1"/>
-      <c r="T22" s="143"/>
-      <c r="U22" s="143"/>
+      <c r="T22" s="156"/>
+      <c r="U22" s="156"/>
     </row>
     <row r="23" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="12">
@@ -3105,24 +3105,24 @@
         <v>4</v>
       </c>
       <c r="C23" s="12"/>
-      <c r="D23" s="137"/>
-      <c r="E23" s="138"/>
-      <c r="F23" s="138"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="139"/>
+      <c r="D23" s="157"/>
+      <c r="E23" s="158"/>
+      <c r="F23" s="158"/>
+      <c r="G23" s="158"/>
+      <c r="H23" s="159"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
       <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M23" s="146"/>
-      <c r="N23" s="146"/>
-      <c r="O23" s="147"/>
+      <c r="M23" s="162"/>
+      <c r="N23" s="162"/>
+      <c r="O23" s="163"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="1"/>
-      <c r="T23" s="143"/>
-      <c r="U23" s="143"/>
+      <c r="T23" s="156"/>
+      <c r="U23" s="156"/>
     </row>
     <row r="24" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="12">
@@ -3130,24 +3130,24 @@
         <v>5</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="137"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="138"/>
-      <c r="H24" s="139"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="158"/>
+      <c r="F24" s="158"/>
+      <c r="G24" s="158"/>
+      <c r="H24" s="159"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="146"/>
-      <c r="N24" s="146"/>
-      <c r="O24" s="147"/>
+      <c r="M24" s="162"/>
+      <c r="N24" s="162"/>
+      <c r="O24" s="163"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="143"/>
-      <c r="U24" s="143"/>
+      <c r="T24" s="156"/>
+      <c r="U24" s="156"/>
     </row>
     <row r="25" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="12">
@@ -3155,24 +3155,24 @@
         <v>6</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="138"/>
-      <c r="F25" s="138"/>
-      <c r="G25" s="138"/>
-      <c r="H25" s="139"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="158"/>
+      <c r="F25" s="158"/>
+      <c r="G25" s="158"/>
+      <c r="H25" s="159"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="148"/>
-      <c r="N25" s="148"/>
-      <c r="O25" s="149"/>
+      <c r="M25" s="164"/>
+      <c r="N25" s="164"/>
+      <c r="O25" s="165"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="1"/>
-      <c r="T25" s="143"/>
-      <c r="U25" s="143"/>
+      <c r="T25" s="156"/>
+      <c r="U25" s="156"/>
     </row>
     <row r="26" spans="2:21" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="12">
@@ -3180,11 +3180,11 @@
         <v>7</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="133"/>
-      <c r="E26" s="134"/>
-      <c r="F26" s="134"/>
-      <c r="G26" s="134"/>
-      <c r="H26" s="135"/>
+      <c r="D26" s="169"/>
+      <c r="E26" s="170"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="171"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
@@ -3203,11 +3203,11 @@
         <v>8</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="133"/>
-      <c r="E27" s="134"/>
-      <c r="F27" s="134"/>
-      <c r="G27" s="134"/>
-      <c r="H27" s="135"/>
+      <c r="D27" s="169"/>
+      <c r="E27" s="170"/>
+      <c r="F27" s="170"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="171"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -3226,11 +3226,11 @@
         <v>9</v>
       </c>
       <c r="C28" s="12"/>
-      <c r="D28" s="133"/>
-      <c r="E28" s="134"/>
-      <c r="F28" s="134"/>
-      <c r="G28" s="134"/>
-      <c r="H28" s="135"/>
+      <c r="D28" s="169"/>
+      <c r="E28" s="170"/>
+      <c r="F28" s="170"/>
+      <c r="G28" s="170"/>
+      <c r="H28" s="171"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -3249,11 +3249,11 @@
         <v>10</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="133"/>
-      <c r="E29" s="134"/>
-      <c r="F29" s="134"/>
-      <c r="G29" s="134"/>
-      <c r="H29" s="135"/>
+      <c r="D29" s="169"/>
+      <c r="E29" s="170"/>
+      <c r="F29" s="170"/>
+      <c r="G29" s="170"/>
+      <c r="H29" s="171"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -3272,11 +3272,11 @@
         <v>11</v>
       </c>
       <c r="C30" s="12"/>
-      <c r="D30" s="133"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="135"/>
+      <c r="D30" s="169"/>
+      <c r="E30" s="170"/>
+      <c r="F30" s="170"/>
+      <c r="G30" s="170"/>
+      <c r="H30" s="171"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -3295,11 +3295,11 @@
         <v>12</v>
       </c>
       <c r="C31" s="12"/>
-      <c r="D31" s="133"/>
-      <c r="E31" s="134"/>
-      <c r="F31" s="134"/>
-      <c r="G31" s="134"/>
-      <c r="H31" s="135"/>
+      <c r="D31" s="169"/>
+      <c r="E31" s="170"/>
+      <c r="F31" s="170"/>
+      <c r="G31" s="170"/>
+      <c r="H31" s="171"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
@@ -3318,11 +3318,11 @@
         <v>13</v>
       </c>
       <c r="C32" s="12"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="134"/>
-      <c r="F32" s="134"/>
-      <c r="G32" s="134"/>
-      <c r="H32" s="135"/>
+      <c r="D32" s="169"/>
+      <c r="E32" s="170"/>
+      <c r="F32" s="170"/>
+      <c r="G32" s="170"/>
+      <c r="H32" s="171"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
@@ -3341,11 +3341,11 @@
         <v>14</v>
       </c>
       <c r="C33" s="12"/>
-      <c r="D33" s="133"/>
-      <c r="E33" s="134"/>
-      <c r="F33" s="134"/>
-      <c r="G33" s="134"/>
-      <c r="H33" s="135"/>
+      <c r="D33" s="169"/>
+      <c r="E33" s="170"/>
+      <c r="F33" s="170"/>
+      <c r="G33" s="170"/>
+      <c r="H33" s="171"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
@@ -3360,11 +3360,11 @@
         <v>15</v>
       </c>
       <c r="C34" s="12"/>
-      <c r="D34" s="137"/>
-      <c r="E34" s="138"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="138"/>
-      <c r="H34" s="139"/>
+      <c r="D34" s="157"/>
+      <c r="E34" s="158"/>
+      <c r="F34" s="158"/>
+      <c r="G34" s="158"/>
+      <c r="H34" s="159"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
@@ -3379,11 +3379,11 @@
         <v>16</v>
       </c>
       <c r="C35" s="12"/>
-      <c r="D35" s="137"/>
-      <c r="E35" s="138"/>
-      <c r="F35" s="138"/>
-      <c r="G35" s="138"/>
-      <c r="H35" s="139"/>
+      <c r="D35" s="157"/>
+      <c r="E35" s="158"/>
+      <c r="F35" s="158"/>
+      <c r="G35" s="158"/>
+      <c r="H35" s="159"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
@@ -3398,11 +3398,11 @@
         <v>17</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="137"/>
-      <c r="E36" s="138"/>
-      <c r="F36" s="138"/>
-      <c r="G36" s="138"/>
-      <c r="H36" s="139"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="158"/>
+      <c r="F36" s="158"/>
+      <c r="G36" s="158"/>
+      <c r="H36" s="159"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
@@ -3417,11 +3417,11 @@
         <v>18</v>
       </c>
       <c r="C37" s="12"/>
-      <c r="D37" s="137"/>
-      <c r="E37" s="138"/>
-      <c r="F37" s="138"/>
-      <c r="G37" s="138"/>
-      <c r="H37" s="139"/>
+      <c r="D37" s="157"/>
+      <c r="E37" s="158"/>
+      <c r="F37" s="158"/>
+      <c r="G37" s="158"/>
+      <c r="H37" s="159"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
@@ -3436,11 +3436,11 @@
         <v>19</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="140"/>
-      <c r="E38" s="141"/>
-      <c r="F38" s="141"/>
-      <c r="G38" s="141"/>
-      <c r="H38" s="142"/>
+      <c r="D38" s="166"/>
+      <c r="E38" s="167"/>
+      <c r="F38" s="167"/>
+      <c r="G38" s="167"/>
+      <c r="H38" s="168"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -3471,10 +3471,10 @@
       <c r="T39" s="3"/>
     </row>
     <row r="40" spans="2:20" s="1" customFormat="1">
-      <c r="B40" s="171" t="s">
+      <c r="B40" s="153" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="171"/>
+      <c r="C40" s="153"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
         <v>8</v>
@@ -3490,14 +3490,14 @@
       </c>
     </row>
     <row r="41" spans="2:20">
-      <c r="B41" s="136"/>
-      <c r="C41" s="136"/>
+      <c r="B41" s="142"/>
+      <c r="C41" s="142"/>
     </row>
     <row r="43" spans="2:20" s="1" customFormat="1">
-      <c r="B43" s="136" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="171"/>
+      <c r="B43" s="142" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="153"/>
       <c r="F43" s="1" t="s">
         <v>5</v>
       </c>
@@ -3512,10 +3512,10 @@
       </c>
     </row>
     <row r="44" spans="2:20" s="1" customFormat="1">
-      <c r="B44" s="136" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="136"/>
+      <c r="B44" s="142" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="142"/>
       <c r="F44" s="1" t="s">
         <v>2</v>
       </c>
@@ -3527,23 +3527,54 @@
       </c>
     </row>
     <row r="45" spans="2:20">
-      <c r="B45" s="158"/>
-      <c r="C45" s="158"/>
-      <c r="D45" s="158"/>
-      <c r="E45" s="158"/>
-      <c r="F45" s="158"/>
-      <c r="G45" s="158"/>
-      <c r="H45" s="158"/>
-      <c r="I45" s="158"/>
-      <c r="J45" s="158"/>
-      <c r="K45" s="158"/>
-      <c r="L45" s="158"/>
-      <c r="M45" s="158"/>
-      <c r="N45" s="158"/>
-      <c r="O45" s="158"/>
+      <c r="B45" s="133"/>
+      <c r="C45" s="133"/>
+      <c r="D45" s="133"/>
+      <c r="E45" s="133"/>
+      <c r="F45" s="133"/>
+      <c r="G45" s="133"/>
+      <c r="H45" s="133"/>
+      <c r="I45" s="133"/>
+      <c r="J45" s="133"/>
+      <c r="K45" s="133"/>
+      <c r="L45" s="133"/>
+      <c r="M45" s="133"/>
+      <c r="N45" s="133"/>
+      <c r="O45" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="T20:U25"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
     <mergeCell ref="B45:O45"/>
     <mergeCell ref="F2:N2"/>
     <mergeCell ref="F3:N3"/>
@@ -3560,37 +3591,6 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="T20:U25"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D36:H36"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D30:H30"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.98425196850393704" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -3605,29 +3605,29 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:Q102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="15"/>
-    <col min="4" max="4" width="10.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="35" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="15"/>
+    <col min="4" max="4" width="10.6640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="15" customWidth="1"/>
     <col min="7" max="7" width="19" style="15" customWidth="1"/>
-    <col min="8" max="9" width="11.42578125" style="15"/>
-    <col min="10" max="10" width="12.85546875" style="15" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="15" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="36" customWidth="1"/>
-    <col min="14" max="14" width="5.85546875" style="15" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="15"/>
+    <col min="8" max="9" width="11.44140625" style="15"/>
+    <col min="10" max="10" width="12.88671875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="15" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="15" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="36" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" style="15" customWidth="1"/>
+    <col min="15" max="16384" width="11.44140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="13.5" thickBot="1"/>
+    <row r="1" spans="2:14" ht="13.8" thickBot="1"/>
     <row r="2" spans="2:14" ht="6" customHeight="1" thickTop="1">
       <c r="B2" s="37"/>
       <c r="C2" s="38"/>
@@ -3646,19 +3646,19 @@
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
       <c r="D3" s="43"/>
-      <c r="E3" s="219" t="s">
+      <c r="E3" s="174" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="219"/>
-      <c r="G3" s="219"/>
-      <c r="H3" s="219"/>
-      <c r="I3" s="219"/>
-      <c r="J3" s="219"/>
-      <c r="K3" s="219"/>
-      <c r="L3" s="220" t="s">
+      <c r="F3" s="174"/>
+      <c r="G3" s="174"/>
+      <c r="H3" s="174"/>
+      <c r="I3" s="174"/>
+      <c r="J3" s="174"/>
+      <c r="K3" s="174"/>
+      <c r="L3" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="221"/>
+      <c r="M3" s="176"/>
       <c r="N3" s="44"/>
     </row>
     <row r="4" spans="2:14">
@@ -3684,95 +3684,95 @@
       <c r="I5" s="51"/>
       <c r="J5" s="51"/>
       <c r="K5" s="53"/>
-      <c r="L5" s="222" t="s">
+      <c r="L5" s="177" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="223"/>
+      <c r="M5" s="178"/>
       <c r="N5" s="54"/>
     </row>
-    <row r="6" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B6" s="224" t="s">
+    <row r="6" spans="2:14" ht="14.4" customHeight="1">
+      <c r="B6" s="179" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="226" t="s">
+      <c r="C6" s="181" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="226"/>
-      <c r="E6" s="226"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="230" t="s">
+      <c r="D6" s="181"/>
+      <c r="E6" s="181"/>
+      <c r="F6" s="182"/>
+      <c r="G6" s="185" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="231"/>
-      <c r="I6" s="231"/>
-      <c r="J6" s="231"/>
-      <c r="K6" s="232"/>
-      <c r="L6" s="233">
+      <c r="H6" s="186"/>
+      <c r="I6" s="186"/>
+      <c r="J6" s="186"/>
+      <c r="K6" s="187"/>
+      <c r="L6" s="188">
         <f>L10</f>
         <v>0</v>
       </c>
-      <c r="M6" s="234"/>
+      <c r="M6" s="189"/>
       <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="225"/>
-      <c r="C7" s="228"/>
-      <c r="D7" s="228"/>
-      <c r="E7" s="228"/>
-      <c r="F7" s="229"/>
-      <c r="G7" s="235">
+      <c r="B7" s="180"/>
+      <c r="C7" s="183"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="183"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="190">
         <f>requi!K20</f>
         <v>0</v>
       </c>
-      <c r="H7" s="236"/>
-      <c r="I7" s="236"/>
-      <c r="J7" s="236"/>
-      <c r="K7" s="237"/>
-      <c r="L7" s="238" t="s">
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="191"/>
+      <c r="K7" s="192"/>
+      <c r="L7" s="193" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="239"/>
+      <c r="M7" s="194"/>
       <c r="N7" s="46"/>
     </row>
-    <row r="8" spans="2:14" ht="12.95" customHeight="1">
-      <c r="B8" s="240" t="s">
+    <row r="8" spans="2:14" ht="12.9" customHeight="1">
+      <c r="B8" s="195" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="241" t="s">
+      <c r="C8" s="196" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="241"/>
-      <c r="E8" s="241"/>
-      <c r="F8" s="242"/>
-      <c r="G8" s="245" t="s">
+      <c r="D8" s="196"/>
+      <c r="E8" s="196"/>
+      <c r="F8" s="197"/>
+      <c r="G8" s="200" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="241"/>
-      <c r="I8" s="241"/>
-      <c r="J8" s="241"/>
-      <c r="K8" s="242"/>
-      <c r="L8" s="247">
+      <c r="H8" s="196"/>
+      <c r="I8" s="196"/>
+      <c r="J8" s="196"/>
+      <c r="K8" s="197"/>
+      <c r="L8" s="202">
         <f>requi!C11</f>
         <v>0</v>
       </c>
-      <c r="M8" s="248"/>
+      <c r="M8" s="203"/>
       <c r="N8" s="55"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="225"/>
-      <c r="C9" s="243"/>
-      <c r="D9" s="243"/>
-      <c r="E9" s="243"/>
-      <c r="F9" s="244"/>
-      <c r="G9" s="246"/>
-      <c r="H9" s="243"/>
-      <c r="I9" s="243"/>
-      <c r="J9" s="243"/>
-      <c r="K9" s="244"/>
-      <c r="L9" s="213" t="s">
+      <c r="B9" s="180"/>
+      <c r="C9" s="198"/>
+      <c r="D9" s="198"/>
+      <c r="E9" s="198"/>
+      <c r="F9" s="199"/>
+      <c r="G9" s="201"/>
+      <c r="H9" s="198"/>
+      <c r="I9" s="198"/>
+      <c r="J9" s="198"/>
+      <c r="K9" s="199"/>
+      <c r="L9" s="204" t="s">
         <v>53</v>
       </c>
-      <c r="M9" s="214"/>
+      <c r="M9" s="205"/>
       <c r="N9" s="46"/>
     </row>
     <row r="10" spans="2:14">
@@ -3788,66 +3788,66 @@
       <c r="G10" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="207">
+      <c r="H10" s="206">
         <f>requi!M20</f>
         <v>0</v>
       </c>
-      <c r="I10" s="207"/>
-      <c r="J10" s="207"/>
-      <c r="K10" s="208"/>
-      <c r="L10" s="209">
+      <c r="I10" s="206"/>
+      <c r="J10" s="206"/>
+      <c r="K10" s="207"/>
+      <c r="L10" s="208">
         <f>requi!O5</f>
         <v>0</v>
       </c>
-      <c r="M10" s="210"/>
+      <c r="M10" s="209"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" spans="2:14">
       <c r="B11" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="211">
+      <c r="C11" s="210">
         <f>requi!C7</f>
         <v>0</v>
       </c>
-      <c r="D11" s="211"/>
-      <c r="E11" s="211"/>
-      <c r="F11" s="212"/>
+      <c r="D11" s="210"/>
+      <c r="E11" s="210"/>
+      <c r="F11" s="211"/>
       <c r="G11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="207" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="207"/>
-      <c r="J11" s="207"/>
-      <c r="K11" s="208"/>
-      <c r="L11" s="213" t="s">
+      <c r="H11" s="206" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="206"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="207"/>
+      <c r="L11" s="204" t="s">
         <v>59</v>
       </c>
-      <c r="M11" s="214"/>
+      <c r="M11" s="205"/>
     </row>
     <row r="12" spans="2:14">
       <c r="B12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="211"/>
-      <c r="D12" s="211"/>
-      <c r="E12" s="211"/>
-      <c r="F12" s="212"/>
+      <c r="C12" s="210"/>
+      <c r="D12" s="210"/>
+      <c r="E12" s="210"/>
+      <c r="F12" s="211"/>
       <c r="G12" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="207" t="s">
-        <v>85</v>
-      </c>
-      <c r="I12" s="207"/>
-      <c r="J12" s="207"/>
-      <c r="K12" s="208"/>
-      <c r="L12" s="215"/>
-      <c r="M12" s="216"/>
-    </row>
-    <row r="13" spans="2:14" ht="16.899999999999999" customHeight="1" thickBot="1">
+      <c r="H12" s="206" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="206"/>
+      <c r="J12" s="206"/>
+      <c r="K12" s="207"/>
+      <c r="L12" s="212"/>
+      <c r="M12" s="213"/>
+    </row>
+    <row r="13" spans="2:14" ht="16.95" customHeight="1" thickBot="1">
       <c r="B13" s="62"/>
       <c r="C13" s="63"/>
       <c r="D13" s="63"/>
@@ -3856,13 +3856,13 @@
       <c r="G13" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="202">
+      <c r="H13" s="215">
         <f>H34</f>
         <v>0</v>
       </c>
-      <c r="I13" s="202"/>
-      <c r="J13" s="202"/>
-      <c r="K13" s="203"/>
+      <c r="I13" s="215"/>
+      <c r="J13" s="215"/>
+      <c r="K13" s="216"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68"/>
       <c r="N13" s="46"/>
@@ -3870,7 +3870,7 @@
     <row r="14" spans="2:14" ht="5.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="2:14" ht="13.5" thickBot="1">
+    <row r="15" spans="2:14" ht="13.8" thickBot="1">
       <c r="B15" s="69" t="s">
         <v>23</v>
       </c>
@@ -3883,14 +3883,14 @@
       <c r="E15" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="204" t="s">
+      <c r="F15" s="217" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="205"/>
-      <c r="H15" s="205"/>
-      <c r="I15" s="205"/>
-      <c r="J15" s="205"/>
-      <c r="K15" s="206"/>
+      <c r="G15" s="218"/>
+      <c r="H15" s="218"/>
+      <c r="I15" s="218"/>
+      <c r="J15" s="218"/>
+      <c r="K15" s="219"/>
       <c r="L15" s="70" t="s">
         <v>63</v>
       </c>
@@ -3899,7 +3899,7 @@
       </c>
       <c r="N15" s="72"/>
     </row>
-    <row r="16" spans="2:14" s="73" customFormat="1" ht="14.45" customHeight="1">
+    <row r="16" spans="2:14" s="73" customFormat="1" ht="14.4" customHeight="1">
       <c r="B16" s="74">
         <v>1</v>
       </c>
@@ -3915,18 +3915,18 @@
         <f>requi!C20</f>
         <v>0</v>
       </c>
-      <c r="F16" s="172">
+      <c r="F16" s="214">
         <f>requi!D20</f>
         <v>0</v>
       </c>
-      <c r="G16" s="172"/>
-      <c r="H16" s="172"/>
-      <c r="I16" s="172"/>
-      <c r="J16" s="172"/>
-      <c r="K16" s="172"/>
+      <c r="G16" s="214"/>
+      <c r="H16" s="214"/>
+      <c r="I16" s="214"/>
+      <c r="J16" s="214"/>
+      <c r="K16" s="214"/>
       <c r="L16" s="75"/>
       <c r="M16" s="76">
-        <f t="shared" ref="M16:M33" si="0">L16*C16</f>
+        <f t="shared" ref="M16:M30" si="0">L16*C16</f>
         <v>0</v>
       </c>
       <c r="N16" s="77"/>
@@ -3947,15 +3947,15 @@
         <f>requi!C21</f>
         <v>0</v>
       </c>
-      <c r="F17" s="172">
+      <c r="F17" s="214">
         <f>requi!D21</f>
         <v>0</v>
       </c>
-      <c r="G17" s="172"/>
-      <c r="H17" s="172"/>
-      <c r="I17" s="172"/>
-      <c r="J17" s="172"/>
-      <c r="K17" s="172"/>
+      <c r="G17" s="214"/>
+      <c r="H17" s="214"/>
+      <c r="I17" s="214"/>
+      <c r="J17" s="214"/>
+      <c r="K17" s="214"/>
       <c r="L17" s="80"/>
       <c r="M17" s="76">
         <f t="shared" si="0"/>
@@ -3979,15 +3979,15 @@
         <f>requi!C22</f>
         <v>0</v>
       </c>
-      <c r="F18" s="172">
+      <c r="F18" s="214">
         <f>requi!D22</f>
         <v>0</v>
       </c>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
-      <c r="K18" s="172"/>
+      <c r="G18" s="214"/>
+      <c r="H18" s="214"/>
+      <c r="I18" s="214"/>
+      <c r="J18" s="214"/>
+      <c r="K18" s="214"/>
       <c r="L18" s="80"/>
       <c r="M18" s="76">
         <f t="shared" si="0"/>
@@ -4011,15 +4011,15 @@
         <f>requi!C23</f>
         <v>0</v>
       </c>
-      <c r="F19" s="172">
+      <c r="F19" s="214">
         <f>requi!D23</f>
         <v>0</v>
       </c>
-      <c r="G19" s="172"/>
-      <c r="H19" s="172"/>
-      <c r="I19" s="172"/>
-      <c r="J19" s="172"/>
-      <c r="K19" s="172"/>
+      <c r="G19" s="214"/>
+      <c r="H19" s="214"/>
+      <c r="I19" s="214"/>
+      <c r="J19" s="214"/>
+      <c r="K19" s="214"/>
       <c r="L19" s="80"/>
       <c r="M19" s="76">
         <f t="shared" si="0"/>
@@ -4043,15 +4043,15 @@
         <f>requi!C24</f>
         <v>0</v>
       </c>
-      <c r="F20" s="172">
+      <c r="F20" s="214">
         <f>requi!D24</f>
         <v>0</v>
       </c>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172"/>
-      <c r="J20" s="172"/>
-      <c r="K20" s="172"/>
+      <c r="G20" s="214"/>
+      <c r="H20" s="214"/>
+      <c r="I20" s="214"/>
+      <c r="J20" s="214"/>
+      <c r="K20" s="214"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76">
         <f t="shared" si="0"/>
@@ -4076,15 +4076,15 @@
         <f>requi!C25</f>
         <v>0</v>
       </c>
-      <c r="F21" s="172">
+      <c r="F21" s="214">
         <f>requi!D25</f>
         <v>0</v>
       </c>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172"/>
-      <c r="J21" s="172"/>
-      <c r="K21" s="172"/>
+      <c r="G21" s="214"/>
+      <c r="H21" s="214"/>
+      <c r="I21" s="214"/>
+      <c r="J21" s="214"/>
+      <c r="K21" s="214"/>
       <c r="L21" s="80"/>
       <c r="M21" s="76">
         <f t="shared" si="0"/>
@@ -4109,15 +4109,15 @@
         <f>requi!C26</f>
         <v>0</v>
       </c>
-      <c r="F22" s="172">
+      <c r="F22" s="214">
         <f>requi!D26</f>
         <v>0</v>
       </c>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172"/>
-      <c r="J22" s="172"/>
-      <c r="K22" s="172"/>
+      <c r="G22" s="214"/>
+      <c r="H22" s="214"/>
+      <c r="I22" s="214"/>
+      <c r="J22" s="214"/>
+      <c r="K22" s="214"/>
       <c r="L22" s="80"/>
       <c r="M22" s="76">
         <f t="shared" si="0"/>
@@ -4142,15 +4142,15 @@
         <f>requi!C27</f>
         <v>0</v>
       </c>
-      <c r="F23" s="172">
+      <c r="F23" s="214">
         <f>requi!D27</f>
         <v>0</v>
       </c>
-      <c r="G23" s="172"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="172"/>
-      <c r="J23" s="172"/>
-      <c r="K23" s="172"/>
+      <c r="G23" s="214"/>
+      <c r="H23" s="214"/>
+      <c r="I23" s="214"/>
+      <c r="J23" s="214"/>
+      <c r="K23" s="214"/>
       <c r="L23" s="80"/>
       <c r="M23" s="76">
         <f t="shared" si="0"/>
@@ -4175,15 +4175,15 @@
         <f>requi!C28</f>
         <v>0</v>
       </c>
-      <c r="F24" s="172">
+      <c r="F24" s="214">
         <f>requi!D28</f>
         <v>0</v>
       </c>
-      <c r="G24" s="172"/>
-      <c r="H24" s="172"/>
-      <c r="I24" s="172"/>
-      <c r="J24" s="172"/>
-      <c r="K24" s="172"/>
+      <c r="G24" s="214"/>
+      <c r="H24" s="214"/>
+      <c r="I24" s="214"/>
+      <c r="J24" s="214"/>
+      <c r="K24" s="214"/>
       <c r="L24" s="80"/>
       <c r="M24" s="76">
         <f t="shared" si="0"/>
@@ -4208,15 +4208,15 @@
         <f>requi!C29</f>
         <v>0</v>
       </c>
-      <c r="F25" s="172">
+      <c r="F25" s="214">
         <f>requi!D29</f>
         <v>0</v>
       </c>
-      <c r="G25" s="172"/>
-      <c r="H25" s="172"/>
-      <c r="I25" s="172"/>
-      <c r="J25" s="172"/>
-      <c r="K25" s="172"/>
+      <c r="G25" s="214"/>
+      <c r="H25" s="214"/>
+      <c r="I25" s="214"/>
+      <c r="J25" s="214"/>
+      <c r="K25" s="214"/>
       <c r="L25" s="80"/>
       <c r="M25" s="76">
         <f t="shared" si="0"/>
@@ -4241,15 +4241,15 @@
         <f>requi!C30</f>
         <v>0</v>
       </c>
-      <c r="F26" s="172">
+      <c r="F26" s="214">
         <f>requi!D30</f>
         <v>0</v>
       </c>
-      <c r="G26" s="172"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="172"/>
-      <c r="J26" s="172"/>
-      <c r="K26" s="172"/>
+      <c r="G26" s="214"/>
+      <c r="H26" s="214"/>
+      <c r="I26" s="214"/>
+      <c r="J26" s="214"/>
+      <c r="K26" s="214"/>
       <c r="L26" s="80"/>
       <c r="M26" s="76">
         <f t="shared" si="0"/>
@@ -4274,15 +4274,15 @@
         <f>requi!C31</f>
         <v>0</v>
       </c>
-      <c r="F27" s="172">
+      <c r="F27" s="214">
         <f>requi!D31</f>
         <v>0</v>
       </c>
-      <c r="G27" s="172"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="172"/>
-      <c r="J27" s="172"/>
-      <c r="K27" s="172"/>
+      <c r="G27" s="214"/>
+      <c r="H27" s="214"/>
+      <c r="I27" s="214"/>
+      <c r="J27" s="214"/>
+      <c r="K27" s="214"/>
       <c r="L27" s="80"/>
       <c r="M27" s="76">
         <f t="shared" si="0"/>
@@ -4306,15 +4306,15 @@
         <f>requi!C32</f>
         <v>0</v>
       </c>
-      <c r="F28" s="172">
+      <c r="F28" s="214">
         <f>requi!D32</f>
         <v>0</v>
       </c>
-      <c r="G28" s="172"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="172"/>
-      <c r="J28" s="172"/>
-      <c r="K28" s="172"/>
+      <c r="G28" s="214"/>
+      <c r="H28" s="214"/>
+      <c r="I28" s="214"/>
+      <c r="J28" s="214"/>
+      <c r="K28" s="214"/>
       <c r="L28" s="80"/>
       <c r="M28" s="76">
         <f t="shared" si="0"/>
@@ -4338,15 +4338,15 @@
         <f>requi!C33</f>
         <v>0</v>
       </c>
-      <c r="F29" s="172">
+      <c r="F29" s="214">
         <f>requi!D33</f>
         <v>0</v>
       </c>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="172"/>
-      <c r="K29" s="172"/>
+      <c r="G29" s="214"/>
+      <c r="H29" s="214"/>
+      <c r="I29" s="214"/>
+      <c r="J29" s="214"/>
+      <c r="K29" s="214"/>
       <c r="L29" s="80"/>
       <c r="M29" s="76">
         <f t="shared" si="0"/>
@@ -4370,15 +4370,15 @@
         <f>requi!C34</f>
         <v>0</v>
       </c>
-      <c r="F30" s="172">
+      <c r="F30" s="214">
         <f>requi!D34</f>
         <v>0</v>
       </c>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="172"/>
-      <c r="J30" s="172"/>
-      <c r="K30" s="172"/>
+      <c r="G30" s="214"/>
+      <c r="H30" s="214"/>
+      <c r="I30" s="214"/>
+      <c r="J30" s="214"/>
+      <c r="K30" s="214"/>
       <c r="L30" s="80"/>
       <c r="M30" s="76">
         <f t="shared" si="0"/>
@@ -4393,12 +4393,12 @@
       <c r="C31" s="129"/>
       <c r="D31" s="129"/>
       <c r="E31" s="129"/>
-      <c r="F31" s="172"/>
-      <c r="G31" s="172"/>
-      <c r="H31" s="172"/>
-      <c r="I31" s="172"/>
-      <c r="J31" s="172"/>
-      <c r="K31" s="172"/>
+      <c r="F31" s="214"/>
+      <c r="G31" s="214"/>
+      <c r="H31" s="214"/>
+      <c r="I31" s="214"/>
+      <c r="J31" s="214"/>
+      <c r="K31" s="214"/>
       <c r="L31" s="80"/>
       <c r="M31" s="76"/>
       <c r="N31" s="81"/>
@@ -4448,10 +4448,10 @@
       <c r="G34" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H34" s="191"/>
-      <c r="I34" s="191"/>
-      <c r="J34" s="191"/>
-      <c r="K34" s="192"/>
+      <c r="H34" s="247"/>
+      <c r="I34" s="247"/>
+      <c r="J34" s="247"/>
+      <c r="K34" s="248"/>
       <c r="L34" s="80"/>
       <c r="M34" s="76"/>
       <c r="N34" s="81"/>
@@ -4467,13 +4467,13 @@
       <c r="G35" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="H35" s="191">
+      <c r="H35" s="247">
         <f>requi!M23</f>
         <v>0</v>
       </c>
-      <c r="I35" s="191"/>
-      <c r="J35" s="191"/>
-      <c r="K35" s="192"/>
+      <c r="I35" s="247"/>
+      <c r="J35" s="247"/>
+      <c r="K35" s="248"/>
       <c r="L35" s="80"/>
       <c r="M35" s="76"/>
       <c r="N35" s="81"/>
@@ -4489,13 +4489,13 @@
       <c r="G36" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="191">
+      <c r="H36" s="247">
         <f>requi!M24</f>
         <v>0</v>
       </c>
-      <c r="I36" s="191"/>
-      <c r="J36" s="191"/>
-      <c r="K36" s="192"/>
+      <c r="I36" s="247"/>
+      <c r="J36" s="247"/>
+      <c r="K36" s="248"/>
       <c r="L36" s="80"/>
       <c r="M36" s="76"/>
       <c r="N36" s="81"/>
@@ -4511,13 +4511,13 @@
       <c r="G37" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H37" s="191">
+      <c r="H37" s="247">
         <f>requi!M25</f>
         <v>0</v>
       </c>
-      <c r="I37" s="191"/>
-      <c r="J37" s="191"/>
-      <c r="K37" s="192"/>
+      <c r="I37" s="247"/>
+      <c r="J37" s="247"/>
+      <c r="K37" s="248"/>
       <c r="L37" s="80"/>
       <c r="M37" s="76"/>
       <c r="N37" s="81"/>
@@ -4533,13 +4533,13 @@
       <c r="G38" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H38" s="191">
+      <c r="H38" s="247">
         <f>requi!M22</f>
         <v>0</v>
       </c>
-      <c r="I38" s="191"/>
-      <c r="J38" s="191"/>
-      <c r="K38" s="192"/>
+      <c r="I38" s="247"/>
+      <c r="J38" s="247"/>
+      <c r="K38" s="248"/>
       <c r="L38" s="80"/>
       <c r="M38" s="76"/>
       <c r="N38" s="81"/>
@@ -4559,31 +4559,31 @@
       <c r="G39" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="191">
+      <c r="H39" s="247">
         <f>requi!M21</f>
         <v>0</v>
       </c>
-      <c r="I39" s="191"/>
-      <c r="J39" s="191"/>
-      <c r="K39" s="192"/>
+      <c r="I39" s="247"/>
+      <c r="J39" s="247"/>
+      <c r="K39" s="248"/>
       <c r="L39" s="80"/>
       <c r="M39" s="76"/>
       <c r="N39" s="81"/>
     </row>
-    <row r="40" spans="2:14" ht="10.9" customHeight="1">
-      <c r="B40" s="179" t="e">
+    <row r="40" spans="2:14" ht="10.95" customHeight="1">
+      <c r="B40" s="235" t="e">
         <f ca="1">PesosMN(M48)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C40" s="180"/>
-      <c r="D40" s="180"/>
-      <c r="E40" s="180"/>
-      <c r="F40" s="180"/>
-      <c r="G40" s="180"/>
-      <c r="H40" s="180"/>
-      <c r="I40" s="180"/>
-      <c r="J40" s="180"/>
-      <c r="K40" s="181"/>
+      <c r="C40" s="236"/>
+      <c r="D40" s="236"/>
+      <c r="E40" s="236"/>
+      <c r="F40" s="236"/>
+      <c r="G40" s="236"/>
+      <c r="H40" s="236"/>
+      <c r="I40" s="236"/>
+      <c r="J40" s="236"/>
+      <c r="K40" s="237"/>
       <c r="L40" s="80"/>
       <c r="M40" s="99" t="s">
         <v>29</v>
@@ -4591,18 +4591,18 @@
       <c r="N40" s="100"/>
     </row>
     <row r="41" spans="2:14">
-      <c r="B41" s="182" t="str">
+      <c r="B41" s="238" t="str">
         <f>C6</f>
         <v>TRITURADOS BASÁLTICOS TEPETLAOXTOC</v>
       </c>
-      <c r="C41" s="183"/>
-      <c r="D41" s="183"/>
-      <c r="E41" s="183"/>
-      <c r="F41" s="183"/>
-      <c r="G41" s="183"/>
-      <c r="H41" s="183"/>
-      <c r="I41" s="183"/>
-      <c r="J41" s="184"/>
+      <c r="C41" s="239"/>
+      <c r="D41" s="239"/>
+      <c r="E41" s="239"/>
+      <c r="F41" s="239"/>
+      <c r="G41" s="239"/>
+      <c r="H41" s="239"/>
+      <c r="I41" s="239"/>
+      <c r="J41" s="240"/>
       <c r="K41" s="86"/>
       <c r="L41" s="80" t="s">
         <v>29</v>
@@ -4613,21 +4613,21 @@
       <c r="N41" s="100"/>
     </row>
     <row r="42" spans="2:14">
-      <c r="B42" s="185" t="s">
+      <c r="B42" s="241" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="186"/>
-      <c r="D42" s="186"/>
-      <c r="E42" s="187" t="s">
+      <c r="C42" s="242"/>
+      <c r="D42" s="242"/>
+      <c r="E42" s="243" t="s">
         <v>68</v>
       </c>
-      <c r="F42" s="188"/>
-      <c r="G42" s="189"/>
-      <c r="H42" s="186" t="s">
+      <c r="F42" s="244"/>
+      <c r="G42" s="245"/>
+      <c r="H42" s="242" t="s">
         <v>69</v>
       </c>
-      <c r="I42" s="186"/>
-      <c r="J42" s="190"/>
+      <c r="I42" s="242"/>
+      <c r="J42" s="246"/>
       <c r="K42" s="86"/>
       <c r="L42" s="80" t="s">
         <v>29</v>
@@ -4653,21 +4653,21 @@
       <c r="N43" s="109"/>
     </row>
     <row r="44" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B44" s="201" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="174"/>
-      <c r="D44" s="174"/>
-      <c r="E44" s="173" t="s">
+      <c r="B44" s="228" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="229"/>
+      <c r="D44" s="229"/>
+      <c r="E44" s="230" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="174"/>
-      <c r="G44" s="175"/>
-      <c r="H44" s="174" t="s">
+      <c r="F44" s="229"/>
+      <c r="G44" s="231"/>
+      <c r="H44" s="229" t="s">
         <v>71</v>
       </c>
-      <c r="I44" s="174"/>
-      <c r="J44" s="175"/>
+      <c r="I44" s="229"/>
+      <c r="J44" s="231"/>
       <c r="K44" s="110"/>
       <c r="L44" s="111" t="s">
         <v>72</v>
@@ -4678,18 +4678,18 @@
       </c>
       <c r="N44" s="113"/>
     </row>
-    <row r="45" spans="2:14" ht="14.45" customHeight="1">
-      <c r="B45" s="176" t="s">
+    <row r="45" spans="2:14" ht="14.4" customHeight="1">
+      <c r="B45" s="232" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="177"/>
-      <c r="D45" s="177"/>
-      <c r="E45" s="177"/>
-      <c r="F45" s="177"/>
-      <c r="G45" s="177"/>
-      <c r="H45" s="177"/>
-      <c r="I45" s="177"/>
-      <c r="J45" s="178"/>
+      <c r="C45" s="233"/>
+      <c r="D45" s="233"/>
+      <c r="E45" s="233"/>
+      <c r="F45" s="233"/>
+      <c r="G45" s="233"/>
+      <c r="H45" s="233"/>
+      <c r="I45" s="233"/>
+      <c r="J45" s="234"/>
       <c r="K45" s="114"/>
       <c r="L45" s="115" t="s">
         <v>74</v>
@@ -4700,7 +4700,7 @@
       </c>
       <c r="N45" s="113"/>
     </row>
-    <row r="46" spans="2:14" ht="13.15" customHeight="1">
+    <row r="46" spans="2:14" ht="13.2" customHeight="1">
       <c r="B46" s="116"/>
       <c r="C46" s="117"/>
       <c r="D46" s="117"/>
@@ -4717,19 +4717,19 @@
       <c r="M46" s="112"/>
       <c r="N46" s="113"/>
     </row>
-    <row r="47" spans="2:14" ht="11.45" customHeight="1">
+    <row r="47" spans="2:14" ht="11.4" customHeight="1">
       <c r="B47" s="121"/>
       <c r="E47" s="122"/>
       <c r="F47" s="123" t="s">
         <v>76</v>
       </c>
       <c r="G47" s="124"/>
-      <c r="H47" s="193">
+      <c r="H47" s="220">
         <f>+G7</f>
         <v>0</v>
       </c>
-      <c r="I47" s="193"/>
-      <c r="J47" s="194"/>
+      <c r="I47" s="220"/>
+      <c r="J47" s="221"/>
       <c r="K47" s="114"/>
       <c r="L47" s="115" t="s">
         <v>77</v>
@@ -4738,21 +4738,21 @@
       <c r="N47" s="113"/>
     </row>
     <row r="48" spans="2:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B48" s="195" t="s">
+      <c r="B48" s="222" t="s">
         <v>78</v>
       </c>
-      <c r="C48" s="196"/>
-      <c r="D48" s="196"/>
-      <c r="E48" s="197" t="s">
+      <c r="C48" s="223"/>
+      <c r="D48" s="223"/>
+      <c r="E48" s="224" t="s">
         <v>79</v>
       </c>
-      <c r="F48" s="198"/>
-      <c r="G48" s="199"/>
-      <c r="H48" s="196" t="s">
+      <c r="F48" s="225"/>
+      <c r="G48" s="226"/>
+      <c r="H48" s="223" t="s">
         <v>80</v>
       </c>
-      <c r="I48" s="196"/>
-      <c r="J48" s="200"/>
+      <c r="I48" s="223"/>
+      <c r="J48" s="227"/>
       <c r="K48" s="125" t="s">
         <v>29</v>
       </c>
@@ -4765,19 +4765,19 @@
       </c>
       <c r="N48" s="113"/>
     </row>
-    <row r="49" spans="2:14" ht="13.5" thickTop="1">
-      <c r="B49" s="217"/>
-      <c r="C49" s="217"/>
-      <c r="D49" s="217"/>
-      <c r="E49" s="217"/>
-      <c r="F49" s="217"/>
-      <c r="G49" s="217"/>
-      <c r="H49" s="217"/>
-      <c r="I49" s="217"/>
-      <c r="J49" s="217"/>
-      <c r="K49" s="217"/>
-      <c r="L49" s="217"/>
-      <c r="M49" s="218"/>
+    <row r="49" spans="2:14" ht="13.8" thickTop="1">
+      <c r="B49" s="172"/>
+      <c r="C49" s="172"/>
+      <c r="D49" s="172"/>
+      <c r="E49" s="172"/>
+      <c r="F49" s="172"/>
+      <c r="G49" s="172"/>
+      <c r="H49" s="172"/>
+      <c r="I49" s="172"/>
+      <c r="J49" s="172"/>
+      <c r="K49" s="172"/>
+      <c r="L49" s="172"/>
+      <c r="M49" s="173"/>
       <c r="N49" s="128"/>
     </row>
     <row r="50" spans="2:14">
@@ -4941,6 +4941,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="B45:J45"/>
+    <mergeCell ref="B40:K40"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="F31:K31"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="F16:K16"/>
+    <mergeCell ref="F17:K17"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="F19:K19"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="F27:K27"/>
+    <mergeCell ref="F28:K28"/>
+    <mergeCell ref="F29:K29"/>
+    <mergeCell ref="F30:K30"/>
+    <mergeCell ref="F21:K21"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="F24:K24"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B49:M49"/>
     <mergeCell ref="E3:K3"/>
     <mergeCell ref="L3:M3"/>
@@ -4957,51 +5002,6 @@
     <mergeCell ref="H8:K9"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="F31:K31"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="F16:K16"/>
-    <mergeCell ref="F17:K17"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="F19:K19"/>
-    <mergeCell ref="F20:K20"/>
-    <mergeCell ref="F27:K27"/>
-    <mergeCell ref="F28:K28"/>
-    <mergeCell ref="F29:K29"/>
-    <mergeCell ref="F30:K30"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="F24:K24"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="F25:K25"/>
-    <mergeCell ref="F26:K26"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="B45:J45"/>
-    <mergeCell ref="B40:K40"/>
-    <mergeCell ref="B41:J41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>